<commit_message>
adding full distances file
</commit_message>
<xml_diff>
--- a/results/generations_report.xlsx
+++ b/results/generations_report.xlsx
@@ -353,94 +353,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>13828.041666666601</c:v>
+                  <c:v>12794.52</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12983.208333333299</c:v>
+                  <c:v>12161.41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13162.333333333299</c:v>
+                  <c:v>12018.16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13080.75</c:v>
+                  <c:v>11864.78</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12775.333333333299</c:v>
+                  <c:v>11829.93</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12411</c:v>
+                  <c:v>11065.85</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11717.666666666601</c:v>
+                  <c:v>10282.370000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11111.541666666601</c:v>
+                  <c:v>10496.83</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10255</c:v>
+                  <c:v>9970.36</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10365.25</c:v>
+                  <c:v>9475.6200000000008</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9738.0833333333303</c:v>
+                  <c:v>9079.2199999999993</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10035.333333333299</c:v>
+                  <c:v>9321.44</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9613.5416666666606</c:v>
+                  <c:v>8838.27</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9312.125</c:v>
+                  <c:v>8347.68</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8543.2083333333303</c:v>
+                  <c:v>8217.4500000000007</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8161.25</c:v>
+                  <c:v>8093.89</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8257.7916666666606</c:v>
+                  <c:v>8226.86</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8506.875</c:v>
+                  <c:v>8677.43</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8092.4583333333303</c:v>
+                  <c:v>8815.9500000000007</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8180.7083333333303</c:v>
+                  <c:v>8516.73</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7884.875</c:v>
+                  <c:v>8171.27</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8016.9166666666597</c:v>
+                  <c:v>7811.86</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7918.3333333333303</c:v>
+                  <c:v>7514.73</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7916.375</c:v>
+                  <c:v>7485.4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7667.2083333333303</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7633.5416666666597</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7608.2083333333303</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7560.375</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7515.375</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7487.25</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>7476</c:v>
@@ -542,94 +542,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>1672.78456670224</c:v>
+                  <c:v>2052.38666668832</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>887.37609365883998</c:v>
+                  <c:v>2020.8509252045201</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1106.7686323507501</c:v>
+                  <c:v>2102.27682630047</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1797.4498196519</c:v>
+                  <c:v>2230.0912384025901</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1417.7277790731</c:v>
+                  <c:v>2178.20374278899</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1413.4037521765199</c:v>
+                  <c:v>1993.5333725573701</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1872.1655390364199</c:v>
+                  <c:v>1932.6366531502999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1381.2958583387799</c:v>
+                  <c:v>2162.08477195044</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1977.3719722567701</c:v>
+                  <c:v>1773.0157332635199</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1045.04151632044</c:v>
+                  <c:v>1476.5283727717499</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1069.8462084441001</c:v>
+                  <c:v>1277.4909125312699</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1261.2557785353799</c:v>
+                  <c:v>1442.98585800415</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>974.19706165157095</c:v>
+                  <c:v>1180.18245924094</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>636.86270841916905</c:v>
+                  <c:v>1023.20727010708</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>727.84911320769095</c:v>
+                  <c:v>825.01190748982503</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>362.45232445109201</c:v>
+                  <c:v>864.71053994964097</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>439.52085456462902</c:v>
+                  <c:v>772.88162120728396</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>613.46212274407503</c:v>
+                  <c:v>1254.51623548681</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>477.57782779063501</c:v>
+                  <c:v>1111.43145875038</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>650.28970974268202</c:v>
+                  <c:v>1074.25901769545</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>322.26067508824798</c:v>
+                  <c:v>1045.2738383313699</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>496.23448058576298</c:v>
+                  <c:v>700.05255545566001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>377.75760158540203</c:v>
+                  <c:v>141.05005175468699</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>538.55909707446801</c:v>
+                  <c:v>65.8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>93.042543659100104</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>70.791347850959497</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>68.193950835506996</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>65.356593967250106</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>61.361505644825897</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>37.312028891498201</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0</c:v>
@@ -731,94 +731,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>16303</c:v>
+                  <c:v>16807</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15231</c:v>
+                  <c:v>17513</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16064</c:v>
+                  <c:v>16569</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16371</c:v>
+                  <c:v>17070</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15269</c:v>
+                  <c:v>16689</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15885</c:v>
+                  <c:v>16149</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16963</c:v>
+                  <c:v>15537</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13991</c:v>
+                  <c:v>15923</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13991</c:v>
+                  <c:v>13847</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12147</c:v>
+                  <c:v>12935</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11931</c:v>
+                  <c:v>12935</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12339</c:v>
+                  <c:v>12180</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12084</c:v>
+                  <c:v>12675</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10429</c:v>
+                  <c:v>11464</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10303</c:v>
+                  <c:v>11171</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9206</c:v>
+                  <c:v>11171</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9585</c:v>
+                  <c:v>10576</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9942</c:v>
+                  <c:v>12146</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9603</c:v>
+                  <c:v>11101</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9882</c:v>
+                  <c:v>11009</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8998</c:v>
+                  <c:v>11813</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9015</c:v>
+                  <c:v>11286</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8998</c:v>
+                  <c:v>8441</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9587</c:v>
+                  <c:v>7946</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7946</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7780</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7780</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7611</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7611</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7611</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>7476</c:v>
@@ -920,79 +920,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>11813</c:v>
+                  <c:v>8399</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11759</c:v>
+                  <c:v>8399</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11540</c:v>
+                  <c:v>7775</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8117</c:v>
+                  <c:v>7775</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10586</c:v>
+                  <c:v>7775</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10471</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9309</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9206</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8086</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8997</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8117</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8622</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8455</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7946</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7662</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7662</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7662</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7887</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7611</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7611</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7611</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7611</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7611</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7611</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7611</c:v>
+                  <c:v>7476</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>7476</c:v>
@@ -2136,16 +2136,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>13828.041666666601</v>
+        <v>12794.52</v>
       </c>
       <c r="C2">
-        <v>1672.78456670224</v>
+        <v>2052.38666668832</v>
       </c>
       <c r="D2">
-        <v>16303</v>
+        <v>16807</v>
       </c>
       <c r="E2">
-        <v>11813</v>
+        <v>8399</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2153,16 +2153,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>12983.208333333299</v>
+        <v>12161.41</v>
       </c>
       <c r="C3">
-        <v>887.37609365883998</v>
+        <v>2020.8509252045201</v>
       </c>
       <c r="D3">
-        <v>15231</v>
+        <v>17513</v>
       </c>
       <c r="E3">
-        <v>11759</v>
+        <v>8399</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2170,16 +2170,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>13162.333333333299</v>
+        <v>12018.16</v>
       </c>
       <c r="C4">
-        <v>1106.7686323507501</v>
+        <v>2102.27682630047</v>
       </c>
       <c r="D4">
-        <v>16064</v>
+        <v>16569</v>
       </c>
       <c r="E4">
-        <v>11540</v>
+        <v>7775</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2187,16 +2187,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>13080.75</v>
+        <v>11864.78</v>
       </c>
       <c r="C5">
-        <v>1797.4498196519</v>
+        <v>2230.0912384025901</v>
       </c>
       <c r="D5">
-        <v>16371</v>
+        <v>17070</v>
       </c>
       <c r="E5">
-        <v>8117</v>
+        <v>7775</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2204,16 +2204,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>12775.333333333299</v>
+        <v>11829.93</v>
       </c>
       <c r="C6">
-        <v>1417.7277790731</v>
+        <v>2178.20374278899</v>
       </c>
       <c r="D6">
-        <v>15269</v>
+        <v>16689</v>
       </c>
       <c r="E6">
-        <v>10586</v>
+        <v>7775</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2221,16 +2221,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>12411</v>
+        <v>11065.85</v>
       </c>
       <c r="C7">
-        <v>1413.4037521765199</v>
+        <v>1993.5333725573701</v>
       </c>
       <c r="D7">
-        <v>15885</v>
+        <v>16149</v>
       </c>
       <c r="E7">
-        <v>10471</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2238,16 +2238,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>11717.666666666601</v>
+        <v>10282.370000000001</v>
       </c>
       <c r="C8">
-        <v>1872.1655390364199</v>
+        <v>1932.6366531502999</v>
       </c>
       <c r="D8">
-        <v>16963</v>
+        <v>15537</v>
       </c>
       <c r="E8">
-        <v>9309</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2255,16 +2255,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>11111.541666666601</v>
+        <v>10496.83</v>
       </c>
       <c r="C9">
-        <v>1381.2958583387799</v>
+        <v>2162.08477195044</v>
       </c>
       <c r="D9">
-        <v>13991</v>
+        <v>15923</v>
       </c>
       <c r="E9">
-        <v>9206</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2272,16 +2272,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>10255</v>
+        <v>9970.36</v>
       </c>
       <c r="C10">
-        <v>1977.3719722567701</v>
+        <v>1773.0157332635199</v>
       </c>
       <c r="D10">
-        <v>13991</v>
+        <v>13847</v>
       </c>
       <c r="E10">
-        <v>8086</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2289,16 +2289,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>10365.25</v>
+        <v>9475.6200000000008</v>
       </c>
       <c r="C11">
-        <v>1045.04151632044</v>
+        <v>1476.5283727717499</v>
       </c>
       <c r="D11">
-        <v>12147</v>
+        <v>12935</v>
       </c>
       <c r="E11">
-        <v>8997</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2306,16 +2306,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>9738.0833333333303</v>
+        <v>9079.2199999999993</v>
       </c>
       <c r="C12">
-        <v>1069.8462084441001</v>
+        <v>1277.4909125312699</v>
       </c>
       <c r="D12">
-        <v>11931</v>
+        <v>12935</v>
       </c>
       <c r="E12">
-        <v>8117</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2323,16 +2323,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>10035.333333333299</v>
+        <v>9321.44</v>
       </c>
       <c r="C13">
-        <v>1261.2557785353799</v>
+        <v>1442.98585800415</v>
       </c>
       <c r="D13">
-        <v>12339</v>
+        <v>12180</v>
       </c>
       <c r="E13">
-        <v>8622</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2340,16 +2340,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>9613.5416666666606</v>
+        <v>8838.27</v>
       </c>
       <c r="C14">
-        <v>974.19706165157095</v>
+        <v>1180.18245924094</v>
       </c>
       <c r="D14">
-        <v>12084</v>
+        <v>12675</v>
       </c>
       <c r="E14">
-        <v>8455</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2357,16 +2357,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>9312.125</v>
+        <v>8347.68</v>
       </c>
       <c r="C15">
-        <v>636.86270841916905</v>
+        <v>1023.20727010708</v>
       </c>
       <c r="D15">
-        <v>10429</v>
+        <v>11464</v>
       </c>
       <c r="E15">
-        <v>7946</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2374,16 +2374,16 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>8543.2083333333303</v>
+        <v>8217.4500000000007</v>
       </c>
       <c r="C16">
-        <v>727.84911320769095</v>
+        <v>825.01190748982503</v>
       </c>
       <c r="D16">
-        <v>10303</v>
+        <v>11171</v>
       </c>
       <c r="E16">
-        <v>7662</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2391,16 +2391,16 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>8161.25</v>
+        <v>8093.89</v>
       </c>
       <c r="C17">
-        <v>362.45232445109201</v>
+        <v>864.71053994964097</v>
       </c>
       <c r="D17">
-        <v>9206</v>
+        <v>11171</v>
       </c>
       <c r="E17">
-        <v>7662</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2408,16 +2408,16 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>8257.7916666666606</v>
+        <v>8226.86</v>
       </c>
       <c r="C18">
-        <v>439.52085456462902</v>
+        <v>772.88162120728396</v>
       </c>
       <c r="D18">
-        <v>9585</v>
+        <v>10576</v>
       </c>
       <c r="E18">
-        <v>7662</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2425,16 +2425,16 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>8506.875</v>
+        <v>8677.43</v>
       </c>
       <c r="C19">
-        <v>613.46212274407503</v>
+        <v>1254.51623548681</v>
       </c>
       <c r="D19">
-        <v>9942</v>
+        <v>12146</v>
       </c>
       <c r="E19">
-        <v>7887</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2442,16 +2442,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>8092.4583333333303</v>
+        <v>8815.9500000000007</v>
       </c>
       <c r="C20">
-        <v>477.57782779063501</v>
+        <v>1111.43145875038</v>
       </c>
       <c r="D20">
-        <v>9603</v>
+        <v>11101</v>
       </c>
       <c r="E20">
-        <v>7611</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2459,16 +2459,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>8180.7083333333303</v>
+        <v>8516.73</v>
       </c>
       <c r="C21">
-        <v>650.28970974268202</v>
+        <v>1074.25901769545</v>
       </c>
       <c r="D21">
-        <v>9882</v>
+        <v>11009</v>
       </c>
       <c r="E21">
-        <v>7611</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2476,16 +2476,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>7884.875</v>
+        <v>8171.27</v>
       </c>
       <c r="C22">
-        <v>322.26067508824798</v>
+        <v>1045.2738383313699</v>
       </c>
       <c r="D22">
-        <v>8998</v>
+        <v>11813</v>
       </c>
       <c r="E22">
-        <v>7611</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2493,16 +2493,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>8016.9166666666597</v>
+        <v>7811.86</v>
       </c>
       <c r="C23">
-        <v>496.23448058576298</v>
+        <v>700.05255545566001</v>
       </c>
       <c r="D23">
-        <v>9015</v>
+        <v>11286</v>
       </c>
       <c r="E23">
-        <v>7611</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2510,16 +2510,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>7918.3333333333303</v>
+        <v>7514.73</v>
       </c>
       <c r="C24">
-        <v>377.75760158540203</v>
+        <v>141.05005175468699</v>
       </c>
       <c r="D24">
-        <v>8998</v>
+        <v>8441</v>
       </c>
       <c r="E24">
-        <v>7611</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2527,16 +2527,16 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>7916.375</v>
+        <v>7485.4</v>
       </c>
       <c r="C25">
-        <v>538.55909707446801</v>
+        <v>65.8</v>
       </c>
       <c r="D25">
-        <v>9587</v>
+        <v>7946</v>
       </c>
       <c r="E25">
-        <v>7611</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2544,16 +2544,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>7667.2083333333303</v>
+        <v>7476</v>
       </c>
       <c r="C26">
-        <v>93.042543659100104</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>7946</v>
+        <v>7476</v>
       </c>
       <c r="E26">
-        <v>7611</v>
+        <v>7476</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2561,13 +2561,13 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>7633.5416666666597</v>
+        <v>7476</v>
       </c>
       <c r="C27">
-        <v>70.791347850959497</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>7780</v>
+        <v>7476</v>
       </c>
       <c r="E27">
         <v>7476</v>
@@ -2578,13 +2578,13 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>7608.2083333333303</v>
+        <v>7476</v>
       </c>
       <c r="C28">
-        <v>68.193950835506996</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>7780</v>
+        <v>7476</v>
       </c>
       <c r="E28">
         <v>7476</v>
@@ -2595,13 +2595,13 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>7560.375</v>
+        <v>7476</v>
       </c>
       <c r="C29">
-        <v>65.356593967250106</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>7611</v>
+        <v>7476</v>
       </c>
       <c r="E29">
         <v>7476</v>
@@ -2612,13 +2612,13 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>7515.375</v>
+        <v>7476</v>
       </c>
       <c r="C30">
-        <v>61.361505644825897</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>7611</v>
+        <v>7476</v>
       </c>
       <c r="E30">
         <v>7476</v>
@@ -2629,13 +2629,13 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>7487.25</v>
+        <v>7476</v>
       </c>
       <c r="C31">
-        <v>37.312028891498201</v>
+        <v>0</v>
       </c>
       <c r="D31">
-        <v>7611</v>
+        <v>7476</v>
       </c>
       <c r="E31">
         <v>7476</v>

</xml_diff>